<commit_message>
Tried to fixed all broken links
</commit_message>
<xml_diff>
--- a/Bus Issue Master.xlsx
+++ b/Bus Issue Master.xlsx
@@ -138,7 +138,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,18 +171,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="166" xfId="0">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="167" xfId="0">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -200,7 +188,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -231,32 +219,15 @@
       </c>
     </row>
     <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="n">
-        <v>52</v>
-      </c>
+      <c r="A2" s="5"/>
       <c r="B2" s="6" t="inlineStr">
         <is>
-          <t>Side panel is out</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>43547</v>
-      </c>
-    </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="8" t="n">
-        <v>55</v>
-      </c>
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="C3" s="10" t="n">
-        <v>43547</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4"/>
+          <t>Emergency button does not work</t>
+        </is>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
@@ -367,50 +338,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
-    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Unit #</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Details</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Date Reported</t>
-        </is>
-      </c>
-    </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Should also work</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>43547</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
+    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Unit #</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Date Reported</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
@@ -662,50 +620,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
-    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Unit #</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Details</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Date Reported</t>
-        </is>
-      </c>
-    </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Leaking</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>43547</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
+    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Unit #</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Date Reported</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
@@ -722,50 +667,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
-    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Unit #</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Details</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Date Reported</t>
-        </is>
-      </c>
-    </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Wand will not hold charge</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>43547</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
+    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Unit #</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Date Reported</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
@@ -782,50 +714,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
-    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Unit #</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Details</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Date Reported</t>
-        </is>
-      </c>
-    </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Vertical cord broken on driver side</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>43548</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
+    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Unit #</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Date Reported</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
@@ -842,50 +761,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
-    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Unit #</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Details</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Date Reported</t>
-        </is>
-      </c>
-    </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Should work</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>43547</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" customWidth="true" width="10"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" customWidth="true" width="48"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" customWidth="true" width="19"/>
+    <col collapsed="false" hidden="false" max="1024" min="4" style="0" customWidth="false" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Unit #</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Date Reported</t>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>

</xml_diff>